<commit_message>
Interfaç adaptada a pantalles grans.
</commit_message>
<xml_diff>
--- a/alumnes_ex.xlsx
+++ b/alumnes_ex.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>SÃ­</t>
+          <t>Sí</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -520,7 +520,11 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Whoaaaaaaaaaaaaaaaa!</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
@@ -1150,6 +1154,3310 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>alumno01</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Paiporta</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '7', 'Documentacion': '5', 'ERP': '9', 'Moviles': '5', 'Multiplataforma': '7', 'Robotica': '5', 'Videojuegos': '6'})</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Whoaaaaaaaaaaaaaaaa!</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>alumno02</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>VALENCIA</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Documentacion': '2', 'ERP': '7', 'Moviles': '2', 'Multiplataforma': '10', 'Robotica': '7', 'Videojuegos': '1'})</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>alumno03</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>AlgemesÃ­</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '1', 'Documentacion': '1', 'ERP': '3', 'Moviles': '10', 'Multiplataforma': '9', 'Robotica': '8', 'Videojuegos': '10'})</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>alumno04</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>AlaquÃ s</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Documentacion': '9', 'ERP': '1', 'Moviles': '1', 'Multiplataforma': '7', 'Robotica': '1', 'Videojuegos': '1'})</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>alumno05</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '9', 'Documentacion': '1', 'ERP': '7', 'Moviles': '5', 'Multiplataforma': '9', 'Robotica': '3', 'Videojuegos': '10'})</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>alumno06</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Requena</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '8', 'Documentacion': '5', 'ERP': '5', 'Moviles': '10', 'Multiplataforma': '10', 'Robotica': '9', 'Videojuegos': '8'})</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>alumno07</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>AlgemesÃ­</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '7', 'Documentacion': '1', 'ERP': '1', 'Moviles': '3', 'Multiplataforma': '7', 'Robotica': '1', 'Videojuegos': '10'})</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>alumno08</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '7', 'Documentacion': '7', 'ERP': '7', 'Moviles': '10', 'Multiplataforma': '7', 'Robotica': '7', 'Videojuegos': '10'})</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>alumno09</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Documentacion': '1', 'ERP': '6', 'Moviles': '10', 'Multiplataforma': '10', 'Robotica': '3', 'Videojuegos': '1'})</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>alumno10</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>BenetÃºsser</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '1', 'Documentacion': '3', 'ERP': '6', 'Moviles': '9', 'Multiplataforma': '8', 'Robotica': '1', 'Videojuegos': '5'})</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>alumno11</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Silla</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '4', 'Documentacion': '8', 'ERP': '8', 'Moviles': '8', 'Multiplataforma': '6', 'Robotica': '4', 'Videojuegos': '1'})</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>alumno12</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Benetusser</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '5', 'Documentacion': '5', 'ERP': '5', 'Moviles': '5', 'Multiplataforma': '5', 'Robotica': '5', 'Videojuegos': '5'})</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>alumno13</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '4', 'Documentacion': '1', 'ERP': '1', 'Moviles': '9', 'Multiplataforma': '9', 'Robotica': '9', 'Videojuegos': '5'})</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>alumno14</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '5', 'Documentacion': '1', 'ERP': '1', 'Moviles': '10', 'Multiplataforma': '8', 'Robotica': '1', 'Videojuegos': '1'})</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>alumno15</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>DAM</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '9', 'Documentacion': '7', 'ERP': '10', 'Moviles': '10', 'Multiplataforma': '10', 'Robotica': '5', 'Videojuegos': '8'})</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>alumno16</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Picassent</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '9', 'Devops': '9', 'Disenyador': '8', 'Documentacion': '9', 'Frontend': '8', 'Fullstack': '9', 'Moviles': '8'})</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>alumno17</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Devops': '6', 'Disenyador': '7', 'Documentacion': '4', 'Frontend': '8', 'Fullstack': '9', 'Moviles': '3'})</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>alumno18</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '8', 'Devops': '3', 'Disenyador': '2', 'Documentacion': '2', 'Frontend': '4', 'Fullstack': '8', 'Moviles': '5'})</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>alumno19</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Devops': '5', 'Disenyador': '8', 'Documentacion': '1', 'Frontend': '10', 'Fullstack': '10', 'Moviles': '10'})</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>alumno20</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Sollana</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '7', 'Devops': '7', 'Disenyador': '10', 'Documentacion': '1', 'Frontend': '10', 'Fullstack': '7', 'Moviles': '7'})</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>alumno21</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Carcaixent</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Devops': '7', 'Disenyador': '5', 'Documentacion': '1', 'Frontend': '5', 'Fullstack': '5', 'Moviles': '1 '})</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>alumno22</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '6', 'Devops': '6', 'Disenyador': '8', 'Documentacion': '6', 'Frontend': '7', 'Fullstack': '7', 'Moviles': '6'})</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>alumno23</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '10', 'Devops': '8', 'Disenyador': '8', 'Documentacion': '8', 'Frontend': '8', 'Fullstack': '7', 'Moviles': '6'})</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>alumno24</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Picassent</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '9', 'Devops': '8', 'Disenyador': '8', 'Documentacion': '6', 'Frontend': '9', 'Fullstack': '10', 'Moviles': '8'})</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>alumno25</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '9', 'Devops': '1', 'Disenyador': '9', 'Documentacion': '1', 'Frontend': '9', 'Fullstack': '9', 'Moviles': '1'})</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>alumno26</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '2', 'Devops': '9', 'Disenyador': '2', 'Documentacion': '7', 'Frontend': '9', 'Fullstack': '8', 'Moviles': '5'})</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>alumno27</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Silla</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '7', 'Devops': '2', 'Disenyador': '10', 'Documentacion': '8', 'Frontend': '7', 'Fullstack': '4', 'Moviles': '6'})</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>alumno28</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '6', 'Devops': '8', 'Disenyador': '4', 'Documentacion': '4', 'Frontend': '7', 'Fullstack': '8', 'Moviles': '9'})</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>alumno29</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Benetusser</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '2', 'Devops': '9', 'Disenyador': '1', 'Documentacion': '2', 'Frontend': '4', 'Fullstack': '6', 'Moviles': '3'})</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>alumno30</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>DAW</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Backend': '5', 'Devops': '2', 'Disenyador': '5', 'Documentacion': '6', 'Frontend': '4', 'Fullstack': '8', 'Moviles': '2'})</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>alumno31</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '8', 'BD': '8', 'Ciberseguridad': '10', 'Consultor': '8', 'Hardware': '7', 'HelpDesk': '9', 'Monitorizador': '10', 'Redes': '8', 'Sistemas': '10'})</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>alumno32</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Sueca</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '9', 'BD': '8', 'Ciberseguridad': '6', 'Consultor': '9', 'Hardware': '10', 'HelpDesk': '4', 'Monitorizador': '10', 'Redes': '8', 'Sistemas': '10'})</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>alumno33</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '10', 'Ciberseguridad': '9', 'Consultor': '7', 'Hardware': '7', 'HelpDesk': '6', 'Monitorizador': '7', 'Redes': '8', 'Sistemas': '10'})</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>alumno34</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '2', 'BD': '2', 'Ciberseguridad': '4', 'Consultor': '3', 'Hardware': '4', 'HelpDesk': '2', 'Monitorizador': '3', 'Redes': '1', 'Sistemas': '3'})</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>alumno35</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>La pobla de Vallbona</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '8', 'Ciberseguridad': '8', 'Consultor': '7', 'Hardware': '8', 'HelpDesk': '7', 'Monitorizador': '6', 'Redes': '6', 'Sistemas': '9'})</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>alumno36</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Sollana</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '7', 'Ciberseguridad': '7', 'Consultor': '7', 'Hardware': '7', 'HelpDesk': '7', 'Monitorizador': '7', 'Redes': '7', 'Sistemas': '7'})</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>alumno37</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>L'Olleria</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '10', 'BD': '9', 'Ciberseguridad': '10', 'Consultor': '10', 'Hardware': '8', 'HelpDesk': '8', 'Monitorizador': '9', 'Redes': '9', 'Sistemas': '9'})</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>alumno38</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '2', 'BD': '7', 'Ciberseguridad': '5', 'Consultor': '3', 'Hardware': '1', 'HelpDesk': '9', 'Monitorizador': '4', 'Redes': '1', 'Sistemas': '3'})</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>alumno39</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '1', 'BD': '2', 'Ciberseguridad': '1', 'Consultor': '2', 'Hardware': '1', 'HelpDesk': '1', 'Monitorizador': '1', 'Redes': '2', 'Sistemas': '2'})</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>alumno40</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '7', 'Ciberseguridad': '9', 'Consultor': '7', 'Hardware': '3', 'HelpDesk': '3', 'Monitorizador': '7', 'Redes': '6', 'Sistemas': '7'})</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>alumno41</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>BenifaiÃ³</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '6', 'Ciberseguridad': '9', 'Consultor': '5', 'Hardware': '8', 'HelpDesk': '6', 'Monitorizador': '8', 'Redes': '5', 'Sistemas': '7'})</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>alumno42</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '2', 'BD': '6', 'Ciberseguridad': '4', 'Consultor': '6', 'Hardware': '4', 'HelpDesk': '6', 'Monitorizador': '5', 'Redes': '4', 'Sistemas': '5'})</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>alumno43</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '10', 'BD': '8', 'Ciberseguridad': '9', 'Consultor': '3', 'Hardware': '5', 'HelpDesk': '6', 'Monitorizador': '7', 'Redes': '5', 'Sistemas': '5'})</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>alumno44</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '7', 'BD': '2', 'Ciberseguridad': '5', 'Consultor': '5', 'Hardware': '10', 'HelpDesk': '2', 'Monitorizador': '8', 'Redes': '7', 'Sistemas': '2'})</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>alumno45</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ASIR</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Auditor': '10', 'BD': '6', 'Ciberseguridad': '3', 'Consultor': '10', 'Hardware': '9', 'HelpDesk': '3', 'Monitorizador': '8', 'Redes': '4', 'Sistemas': '2'})</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>alumno46</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '5', 'HelpDesk': '2', 'Instalador': '2', 'Tecnico': '2'})</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>alumno47</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Paiporta</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '8', 'HelpDesk': '2', 'Instalador': '6', 'Tecnico': '6'})</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>alumno48</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Sollana</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '1', 'HelpDesk': '6', 'Instalador': '5', 'Tecnico': '3'})</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>alumno49</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '4', 'HelpDesk': '5', 'Instalador': '8', 'Tecnico': '5'})</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>alumno50</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Silla</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '6', 'HelpDesk': '1', 'Instalador': '3', 'Tecnico': '2'})</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>alumno51</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Silla</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '1', 'HelpDesk': '8', 'Instalador': '4', 'Tecnico': '1'})</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>alumno52</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '6', 'HelpDesk': '3', 'Instalador': '3', 'Tecnico': '7'})</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>alumno53</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '7', 'HelpDesk': '4', 'Instalador': '7', 'Tecnico': '8'})</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>alumno54</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '3', 'HelpDesk': '9', 'Instalador': '10', 'Tecnico': '5'})</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>alumno55</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '8', 'HelpDesk': '6', 'Instalador': '4', 'Tecnico': '9'})</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>alumno56</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '10', 'HelpDesk': '10', 'Instalador': '4', 'Tecnico': '5'})</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>alumno57</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '5', 'HelpDesk': '3', 'Instalador': '5', 'Tecnico': '6'})</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>alumno58</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '4', 'HelpDesk': '8', 'Instalador': '9', 'Tecnico': '9'})</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>alumno59</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Picassent</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '7', 'HelpDesk': '5', 'Instalador': '10', 'Tecnico': '6'})</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>alumno60</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '9', 'HelpDesk': '9', 'Instalador': '1', 'Tecnico': '4'})</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>alumno46</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '5', 'HelpDesk': '2', 'Instalador': '2', 'Tecnico': '2'})</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>alumno47</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Paiporta</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '8', 'HelpDesk': '2', 'Instalador': '6', 'Tecnico': '6'})</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>alumno48</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Sollana</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '1', 'HelpDesk': '6', 'Instalador': '5', 'Tecnico': '3'})</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>alumno49</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '4', 'HelpDesk': '5', 'Instalador': '8', 'Tecnico': '5'})</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>alumno50</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Silla</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '6', 'HelpDesk': '1', 'Instalador': '3', 'Tecnico': '2'})</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>alumno51</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Silla</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '1', 'HelpDesk': '8', 'Instalador': '4', 'Tecnico': '1'})</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>alumno52</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '6', 'HelpDesk': '3', 'Instalador': '3', 'Tecnico': '7'})</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>alumno53</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '7', 'HelpDesk': '4', 'Instalador': '7', 'Tecnico': '8'})</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>alumno54</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '3', 'HelpDesk': '9', 'Instalador': '10', 'Tecnico': '5'})</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>alumno55</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '8', 'HelpDesk': '6', 'Instalador': '4', 'Tecnico': '9'})</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>alumno56</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>SÃ­</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '10', 'HelpDesk': '10', 'Instalador': '4', 'Tecnico': '5'})</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>alumno57</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Alginet</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '5', 'HelpDesk': '3', 'Instalador': '5', 'Tecnico': '6'})</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>alumno58</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Albal</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '4', 'HelpDesk': '8', 'Instalador': '9', 'Tecnico': '9'})</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>alumno59</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Picassent</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '7', 'HelpDesk': '5', 'Instalador': '10', 'Tecnico': '6'})</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>alumno60</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>TSMR</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Catarroja</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {'Asesor': '9', 'HelpDesk': '9', 'Instalador': '1', 'Tecnico': '4'})</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>DefaultMunch(None, {})</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>